<commit_message>
fixed works and loadDatabase
</commit_message>
<xml_diff>
--- a/data/Excel Format/relations/Works.xlsx
+++ b/data/Excel Format/relations/Works.xlsx
@@ -11,15 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="14">
   <si>
     <t>student_ID</t>
   </si>
   <si>
     <t>company_ID</t>
-  </si>
-  <si>
-    <t>facility_ID</t>
   </si>
   <si>
     <t>job_ID</t>
@@ -28,38 +25,41 @@
     <t>term</t>
   </si>
   <si>
-    <t>start_date</t>
+    <t>semester</t>
   </si>
   <si>
-    <t>end_date</t>
+    <t>year</t>
   </si>
   <si>
-    <t>2B</t>
+    <t>Coop 1</t>
   </si>
   <si>
-    <t>3A</t>
+    <t>Spring</t>
   </si>
   <si>
-    <t>4A</t>
+    <t>Fall</t>
   </si>
   <si>
-    <t>2A</t>
+    <t>Winter</t>
   </si>
   <si>
-    <t>3B</t>
+    <t>Coop 2</t>
   </si>
   <si>
-    <t>1B</t>
+    <t>Coop 3</t>
   </si>
   <si>
-    <t>4B</t>
+    <t>Coop 4</t>
+  </si>
+  <si>
+    <t>Coop1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -69,12 +69,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -82,9 +76,9 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,38 +89,31 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <bottom style="thin">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -346,12 +333,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="8.71"/>
     <col customWidth="1" min="2" max="2" width="18.86"/>
-    <col customWidth="1" min="3" max="3" width="17.14"/>
-    <col customWidth="1" min="4" max="4" width="16.71"/>
-    <col customWidth="1" min="5" max="5" width="17.14"/>
-    <col customWidth="1" min="6" max="7" width="15.71"/>
-    <col customWidth="1" min="8" max="8" width="16.0"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col customWidth="1" min="3" max="4" width="17.14"/>
+    <col customWidth="1" min="5" max="6" width="15.71"/>
+    <col customWidth="1" min="7" max="7" width="16.0"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -367,608 +351,1733 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1">
-        <v>1.976751E7</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="2" t="s">
+        <v>7.356463E7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>16.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3">
-        <v>32874.0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>33239.0</v>
+      <c r="G3" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1">
-        <v>8.3950021E7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D4" s="1">
+        <v>5.1458338E7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>57.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1">
+        <v>4.5453885E7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>57.0</v>
+      </c>
+      <c r="D5" s="4">
         <v>2.0</v>
       </c>
-      <c r="E4" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3">
-        <v>33604.0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>33970.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4">
-        <v>1.0871349E7</v>
-      </c>
-      <c r="C5" s="4">
-        <v>57.0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="6">
-        <v>36526.0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>36618.0</v>
+        <v>2022.0</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="4">
-        <v>6.2389417E7</v>
-      </c>
-      <c r="C6" s="4">
-        <v>57.0</v>
+        <v>4.5453885E7</v>
+      </c>
+      <c r="C6" s="3">
+        <v>13.0</v>
       </c>
       <c r="D6" s="4">
         <v>1.0</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1">
+        <v>7.9689206E7</v>
+      </c>
+      <c r="C7" s="3">
+        <v>61.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1">
+        <v>7.9689206E7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>61.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1">
+        <v>9.126056E7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>62.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="1">
+        <v>9.126056E7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>91.0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="1">
+        <v>6.0653931E7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>92.0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="1">
+        <v>2.2779613E7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="1">
+        <v>1.3336678E7</v>
+      </c>
+      <c r="C13" s="3">
+        <v>21.0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="1">
+        <v>2.1217676E7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>22.0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="1">
+        <v>3.4566543E7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>23.0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="1">
+        <v>3.4566543E7</v>
+      </c>
+      <c r="C16" s="3">
+        <v>23.0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="1">
+        <v>3.7486905E7</v>
+      </c>
+      <c r="C17" s="3">
+        <v>59.0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="1">
+        <v>3.7486905E7</v>
+      </c>
+      <c r="C18" s="3">
+        <v>60.0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="1">
+        <v>9.2514073E7</v>
+      </c>
+      <c r="C19" s="3">
+        <v>61.0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="1">
+        <v>9.2514073E7</v>
+      </c>
+      <c r="C20" s="3">
+        <v>61.0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="1">
+        <v>1.0871349E7</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="4">
+        <v>2020.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="1">
+        <v>1.0871349E7</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="4">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="1">
+        <v>2.9586401E7</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="1">
+        <v>2.9586401E7</v>
+      </c>
+      <c r="C24" s="4">
         <v>4.0</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6">
-        <v>36526.0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>36618.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="4">
-        <v>2.9586401E7</v>
-      </c>
-      <c r="C7" s="4">
-        <v>58.0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="D24" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="6">
-        <v>36526.0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>36618.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="4">
-        <v>5.4173986E7</v>
-      </c>
-      <c r="C8" s="4">
-        <v>59.0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="G24" s="4">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="1">
+        <v>7.5628493E7</v>
+      </c>
+      <c r="C25" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="6">
+        <v>2020.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="1">
+        <v>7.5628493E7</v>
+      </c>
+      <c r="C26" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="6">
-        <v>36895.0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>36986.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4">
-        <v>7.5628493E7</v>
-      </c>
-      <c r="C9" s="4">
-        <v>60.0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="6">
-        <v>36895.0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>36986.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="4">
-        <v>2.3849065E7</v>
-      </c>
-      <c r="C10" s="4">
-        <v>61.0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="6">
-        <v>36895.0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>36986.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="4">
+      <c r="G26" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="1">
         <v>9.6017348E7</v>
       </c>
-      <c r="C11" s="4">
-        <v>61.0</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C27" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="6">
+        <v>2020.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="3">
+        <v>9.6017348E7</v>
+      </c>
+      <c r="C28" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="3">
+        <v>9.6017348E7</v>
+      </c>
+      <c r="C29" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="3">
+        <v>9.6017348E7</v>
+      </c>
+      <c r="C30" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="6">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="1">
+        <v>6.5971234E7</v>
+      </c>
+      <c r="C31" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="6">
+        <v>2020.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="1">
+        <v>6.5971234E7</v>
+      </c>
+      <c r="C32" s="4">
+        <v>11.0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" s="1">
+        <v>6.5971234E7</v>
+      </c>
+      <c r="C33" s="4">
+        <v>12.0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="6">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="1">
+        <v>7.1420935E7</v>
+      </c>
+      <c r="C34" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" s="1">
+        <v>7.1420935E7</v>
+      </c>
+      <c r="C35" s="4">
+        <v>14.0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="6">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" s="1">
+        <v>3.9827615E7</v>
+      </c>
+      <c r="C36" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="1">
+        <v>3.9827615E7</v>
+      </c>
+      <c r="C37" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="D37" s="4">
         <v>2.0</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="6">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="1">
+        <v>2.8349567E7</v>
+      </c>
+      <c r="C38" s="4">
+        <v>17.0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="1">
+        <v>2.8349567E7</v>
+      </c>
+      <c r="C39" s="4">
+        <v>18.0</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="6">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="B40" s="1">
+        <v>7.2819365E7</v>
+      </c>
+      <c r="C40" s="4">
+        <v>19.0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="B41" s="1">
+        <v>7.2819365E7</v>
+      </c>
+      <c r="C41" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="B42" s="1">
+        <v>1.837294E7</v>
+      </c>
+      <c r="C42" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="B43" s="1">
+        <v>1.837294E7</v>
+      </c>
+      <c r="C43" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="D43" s="4">
         <v>2.0</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="6">
-        <v>36895.0</v>
-      </c>
-      <c r="H11" s="6">
-        <v>36986.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="4">
-        <v>5.2468719E7</v>
-      </c>
-      <c r="C12" s="4">
-        <v>62.0</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F12" s="5" t="s">
+      <c r="E43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="B44" s="1">
+        <v>2.837491E7</v>
+      </c>
+      <c r="C44" s="5">
+        <v>22.0</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="6">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="B45" s="1">
+        <v>2.837491E7</v>
+      </c>
+      <c r="C45" s="5">
+        <v>22.0</v>
+      </c>
+      <c r="D45" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="B46" s="1">
+        <v>8.5719236E7</v>
+      </c>
+      <c r="C46" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="D46" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="5">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="B47" s="1">
+        <v>8.5719236E7</v>
+      </c>
+      <c r="C47" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="D47" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="5">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="B48" s="1">
+        <v>8.5719236E7</v>
+      </c>
+      <c r="C48" s="5">
+        <v>25.0</v>
+      </c>
+      <c r="D48" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="6">
-        <v>37014.0</v>
-      </c>
-      <c r="H12" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="4">
-        <v>2.837491E7</v>
-      </c>
-      <c r="C13" s="4">
-        <v>88.0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="F48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="B49" s="1">
+        <v>1.0293847E7</v>
+      </c>
+      <c r="C49" s="5">
+        <v>26.0</v>
+      </c>
+      <c r="D49" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="B50" s="1">
+        <v>1.0293847E7</v>
+      </c>
+      <c r="C50" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="B51" s="1">
+        <v>1.6273849E7</v>
+      </c>
+      <c r="C51" s="5">
+        <v>28.0</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="5">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="B52" s="1">
+        <v>1.6273849E7</v>
+      </c>
+      <c r="C52" s="5">
+        <v>29.0</v>
+      </c>
+      <c r="D52" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="5">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="B53" s="1">
+        <v>1.6273849E7</v>
+      </c>
+      <c r="C53" s="5">
+        <v>30.0</v>
+      </c>
+      <c r="D53" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="6">
-        <v>37014.0</v>
-      </c>
-      <c r="H13" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="4">
-        <v>1.8472039E7</v>
-      </c>
-      <c r="C14" s="4">
-        <v>89.0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="F53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="B54" s="1">
+        <v>8.5719263E7</v>
+      </c>
+      <c r="C54" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="D54" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="B55" s="1">
+        <v>1.7482936E7</v>
+      </c>
+      <c r="C55" s="5">
+        <v>32.0</v>
+      </c>
+      <c r="D55" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="B56" s="1">
+        <v>3.8491725E7</v>
+      </c>
+      <c r="C56" s="5">
+        <v>33.0</v>
+      </c>
+      <c r="D56" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="5">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="B57" s="1">
+        <v>3.8491725E7</v>
+      </c>
+      <c r="C57" s="5">
+        <v>34.0</v>
+      </c>
+      <c r="D57" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="5">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="B58" s="1">
+        <v>3.8491725E7</v>
+      </c>
+      <c r="C58" s="5">
+        <v>35.0</v>
+      </c>
+      <c r="D58" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="6">
-        <v>37014.0</v>
-      </c>
-      <c r="H14" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="4">
-        <v>8.5719236E7</v>
-      </c>
-      <c r="C15" s="4">
-        <v>90.0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="6">
-        <v>37014.0</v>
-      </c>
-      <c r="H15" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="4">
-        <v>4.9283617E7</v>
-      </c>
-      <c r="C16" s="4">
-        <v>91.0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="F58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="B59" s="3">
+        <v>2.9384617E7</v>
+      </c>
+      <c r="C59" s="5">
+        <v>36.0</v>
+      </c>
+      <c r="D59" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="5">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="B60" s="3">
+        <v>2.9384617E7</v>
+      </c>
+      <c r="C60" s="5">
+        <v>36.0</v>
+      </c>
+      <c r="D60" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="5">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="B61" s="3">
+        <v>2.9384617E7</v>
+      </c>
+      <c r="C61" s="5">
+        <v>37.0</v>
+      </c>
+      <c r="D61" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="6">
-        <v>37014.0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="4">
-        <v>2.837461E7</v>
-      </c>
-      <c r="C17" s="4">
-        <v>92.0</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="F61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="B62" s="1">
+        <v>4.9283651E7</v>
+      </c>
+      <c r="C62" s="5">
+        <v>38.0</v>
+      </c>
+      <c r="D62" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="B63" s="1">
+        <v>7.8901234E7</v>
+      </c>
+      <c r="C63" s="5">
+        <v>39.0</v>
+      </c>
+      <c r="D63" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="B64" s="1">
+        <v>7.8901234E7</v>
+      </c>
+      <c r="C64" s="5">
+        <v>40.0</v>
+      </c>
+      <c r="D64" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="B65" s="1">
+        <v>8.9012345E7</v>
+      </c>
+      <c r="C65" s="5">
+        <v>41.0</v>
+      </c>
+      <c r="D65" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="B66" s="1">
+        <v>8.9012345E7</v>
+      </c>
+      <c r="C66" s="5">
+        <v>41.0</v>
+      </c>
+      <c r="D66" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="B67" s="1">
+        <v>9.0123456E7</v>
+      </c>
+      <c r="C67" s="5">
+        <v>42.0</v>
+      </c>
+      <c r="D67" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="B68" s="1">
+        <v>9.0123456E7</v>
+      </c>
+      <c r="C68" s="5">
+        <v>43.0</v>
+      </c>
+      <c r="D68" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="69" ht="15.75" customHeight="1">
+      <c r="B69" s="1">
+        <v>6.6667777E7</v>
+      </c>
+      <c r="C69" s="5">
+        <v>44.0</v>
+      </c>
+      <c r="D69" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="B70" s="1">
+        <v>6.6667777E7</v>
+      </c>
+      <c r="C70" s="5">
+        <v>45.0</v>
+      </c>
+      <c r="D70" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="71" ht="15.75" customHeight="1">
+      <c r="B71" s="1">
+        <v>7.7778888E7</v>
+      </c>
+      <c r="C71" s="5">
+        <v>46.0</v>
+      </c>
+      <c r="D71" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="B72" s="1">
+        <v>7.7778888E7</v>
+      </c>
+      <c r="C72" s="5">
+        <v>47.0</v>
+      </c>
+      <c r="D72" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="73" ht="15.75" customHeight="1">
+      <c r="B73" s="1">
+        <v>8.8889999E7</v>
+      </c>
+      <c r="C73" s="5">
+        <v>48.0</v>
+      </c>
+      <c r="D73" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="74" ht="15.75" customHeight="1">
+      <c r="B74" s="1">
+        <v>8.8889999E7</v>
+      </c>
+      <c r="C74" s="5">
+        <v>49.0</v>
+      </c>
+      <c r="D74" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="B75" s="1">
+        <v>9.999E7</v>
+      </c>
+      <c r="C75" s="5">
+        <v>50.0</v>
+      </c>
+      <c r="D75" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="76" ht="15.75" customHeight="1">
+      <c r="B76" s="1">
+        <v>9.999E7</v>
+      </c>
+      <c r="C76" s="5">
+        <v>51.0</v>
+      </c>
+      <c r="D76" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="77" ht="15.75" customHeight="1">
+      <c r="B77" s="1">
+        <v>1.1112222E7</v>
+      </c>
+      <c r="C77" s="5">
+        <v>71.0</v>
+      </c>
+      <c r="D77" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="78" ht="15.75" customHeight="1">
+      <c r="B78" s="1">
+        <v>1.1112222E7</v>
+      </c>
+      <c r="C78" s="5">
+        <v>72.0</v>
+      </c>
+      <c r="D78" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="79" ht="15.75" customHeight="1">
+      <c r="B79" s="2">
+        <v>2.2213333E7</v>
+      </c>
+      <c r="C79" s="5">
+        <v>73.0</v>
+      </c>
+      <c r="D79" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="B80" s="2">
+        <v>2.2213333E7</v>
+      </c>
+      <c r="C80" s="5">
+        <v>74.0</v>
+      </c>
+      <c r="D80" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="B81" s="1">
+        <v>1.570238E7</v>
+      </c>
+      <c r="C81" s="5">
+        <v>76.0</v>
+      </c>
+      <c r="D81" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="B82" s="1">
+        <v>1.570238E7</v>
+      </c>
+      <c r="C82" s="5">
+        <v>77.0</v>
+      </c>
+      <c r="D82" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G82" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="B83" s="1">
+        <v>1.9073284E7</v>
+      </c>
+      <c r="C83" s="5">
+        <v>78.0</v>
+      </c>
+      <c r="D83" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="B84" s="1">
+        <v>1.9073284E7</v>
+      </c>
+      <c r="C84" s="5">
+        <v>79.0</v>
+      </c>
+      <c r="D84" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G84" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="B85" s="1">
+        <v>1.7829051E7</v>
+      </c>
+      <c r="C85" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="D85" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G85" s="5">
+        <v>2020.0</v>
+      </c>
+    </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="B86" s="1">
+        <v>1.7829051E7</v>
+      </c>
+      <c r="C86" s="5">
+        <v>81.0</v>
+      </c>
+      <c r="D86" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G86" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="B87" s="1">
+        <v>1.7829051E7</v>
+      </c>
+      <c r="C87" s="5">
+        <v>82.0</v>
+      </c>
+      <c r="D87" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87" s="5">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="88" ht="15.75" customHeight="1">
+      <c r="B88" s="1">
+        <v>1.7829051E7</v>
+      </c>
+      <c r="C88" s="5">
+        <v>83.0</v>
+      </c>
+      <c r="D88" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="6">
-        <v>37014.0</v>
-      </c>
-      <c r="H17" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="4">
-        <v>2.1987654E7</v>
-      </c>
-      <c r="C18" s="4">
-        <v>13.0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E18" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="6">
-        <v>40666.0</v>
-      </c>
-      <c r="H18" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="4">
-        <v>2.0654321E7</v>
-      </c>
-      <c r="C19" s="4">
-        <v>14.0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="6">
-        <v>40666.0</v>
-      </c>
-      <c r="H19" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="4">
-        <v>2.1345678E7</v>
-      </c>
-      <c r="C20" s="4">
-        <v>15.0</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="6">
-        <v>40666.0</v>
-      </c>
-      <c r="H20" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="4">
-        <v>1.1111222E7</v>
-      </c>
-      <c r="C21" s="4">
-        <v>16.0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="6">
-        <v>40666.0</v>
-      </c>
-      <c r="H21" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="4">
-        <v>2.2223333E7</v>
-      </c>
-      <c r="C22" s="4">
-        <v>17.0</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="6">
-        <v>40666.0</v>
-      </c>
-      <c r="H22" s="6">
-        <v>37127.0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="4">
-        <v>2.1479513E7</v>
-      </c>
-      <c r="C23" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E23" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="6">
-        <v>44441.0</v>
-      </c>
-      <c r="H23" s="6">
-        <v>44553.0</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="4">
-        <v>1.570238E7</v>
-      </c>
-      <c r="C24" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E24" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="6">
-        <v>44441.0</v>
-      </c>
-      <c r="H24" s="6">
-        <v>44553.0</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="4">
-        <v>1.9073284E7</v>
-      </c>
-      <c r="C25" s="4">
-        <v>23.0</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E25" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="6">
-        <v>44441.0</v>
-      </c>
-      <c r="H25" s="6">
-        <v>44553.0</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
+      <c r="F88" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G88" s="5">
+        <v>2023.0</v>
+      </c>
+    </row>
     <row r="89" ht="15.75" customHeight="1"/>
     <row r="90" ht="15.75" customHeight="1"/>
     <row r="91" ht="15.75" customHeight="1"/>
@@ -1881,6 +2990,25 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
+    <row r="1019" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>